<commit_message>
feat: login admin component
</commit_message>
<xml_diff>
--- a/_todo-list.xlsx
+++ b/_todo-list.xlsx
@@ -644,13 +644,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G90"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="D90" sqref="D90"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="46.85546875" customWidth="1"/>
+    <col min="1" max="1" width="49.28515625" customWidth="1"/>
     <col min="2" max="2" width="81.5703125" customWidth="1"/>
     <col min="3" max="3" width="11.42578125" customWidth="1"/>
     <col min="4" max="4" width="10.42578125" customWidth="1"/>
@@ -707,14 +707,14 @@
         <v>10</v>
       </c>
       <c r="E3">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="F3">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="G3">
         <f>(100-F3)</f>
-        <v>0</v>
+        <v>100</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -731,14 +731,14 @@
         <v>10</v>
       </c>
       <c r="E4">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F4">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="G4">
         <f t="shared" ref="G4:G68" si="0">(100-F4)</f>
-        <v>0</v>
+        <v>100</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -755,14 +755,14 @@
         <v>10</v>
       </c>
       <c r="E5">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F5">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="G5">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>100</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -779,14 +779,14 @@
         <v>5</v>
       </c>
       <c r="E6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F6">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="G6">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>100</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -2297,7 +2297,7 @@
         <v>100</v>
       </c>
       <c r="G69">
-        <f t="shared" ref="G69:G81" si="1">(100-F69)</f>
+        <f t="shared" ref="G69:G76" si="1">(100-F69)</f>
         <v>0</v>
       </c>
     </row>
@@ -2489,7 +2489,7 @@
         <v>100</v>
       </c>
       <c r="G77">
-        <f>(100-F77)</f>
+        <f t="shared" ref="G77:G82" si="2">(100-F77)</f>
         <v>0</v>
       </c>
     </row>
@@ -2513,7 +2513,7 @@
         <v>100</v>
       </c>
       <c r="G78">
-        <f>(100-F78)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -2537,7 +2537,7 @@
         <v>100</v>
       </c>
       <c r="G79">
-        <f>(100-F79)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -2561,7 +2561,7 @@
         <v>100</v>
       </c>
       <c r="G80">
-        <f>(100-F80)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -2585,7 +2585,7 @@
         <v>100</v>
       </c>
       <c r="G81">
-        <f>(100-F81)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -2609,7 +2609,7 @@
         <v>100</v>
       </c>
       <c r="G82">
-        <f>(100-F82)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -2633,7 +2633,7 @@
         <v>100</v>
       </c>
       <c r="G83">
-        <f t="shared" ref="G83:G89" si="2">(100-F83)</f>
+        <f t="shared" ref="G83:G89" si="3">(100-F83)</f>
         <v>0</v>
       </c>
     </row>
@@ -2657,7 +2657,7 @@
         <v>100</v>
       </c>
       <c r="G84">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -2681,7 +2681,7 @@
         <v>100</v>
       </c>
       <c r="G85">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -2705,7 +2705,7 @@
         <v>100</v>
       </c>
       <c r="G86">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -2729,7 +2729,7 @@
         <v>100</v>
       </c>
       <c r="G87">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -2753,7 +2753,7 @@
         <v>100</v>
       </c>
       <c r="G88">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -2777,7 +2777,7 @@
         <v>100</v>
       </c>
       <c r="G89">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
feat: db reset and equipe login
</commit_message>
<xml_diff>
--- a/_todo-list.xlsx
+++ b/_todo-list.xlsx
@@ -645,7 +645,7 @@
   <dimension ref="A1:G90"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -803,14 +803,14 @@
         <v>15</v>
       </c>
       <c r="E7">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="F7">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="G7">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>100</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -827,14 +827,14 @@
         <v>10</v>
       </c>
       <c r="E8">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F8">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="G8">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>100</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
@@ -851,14 +851,14 @@
         <v>10</v>
       </c>
       <c r="E9">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="F9">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="G9">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>100</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
@@ -875,14 +875,14 @@
         <v>15</v>
       </c>
       <c r="E10">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F10">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="G10">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>100</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
@@ -899,14 +899,14 @@
         <v>10</v>
       </c>
       <c r="E11">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F11">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="G11">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>100</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
[FIX] assign multiples coureurs to etape
</commit_message>
<xml_diff>
--- a/_todo-list.xlsx
+++ b/_todo-list.xlsx
@@ -644,8 +644,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G90"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="F27" sqref="F27"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="B44" sqref="B44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1283,14 +1283,14 @@
         <v>10</v>
       </c>
       <c r="E27">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="F27">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="G27">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>100</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
@@ -1307,14 +1307,14 @@
         <v>10</v>
       </c>
       <c r="E28">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="F28">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="G28">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>100</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
@@ -1331,14 +1331,14 @@
         <v>10</v>
       </c>
       <c r="E29">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="F29">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="G29">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>100</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
@@ -1355,14 +1355,14 @@
         <v>15</v>
       </c>
       <c r="E30">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="F30">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="G30">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>100</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
@@ -1379,14 +1379,14 @@
         <v>5</v>
       </c>
       <c r="E31">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="F31">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="G31">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>100</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
@@ -1403,14 +1403,14 @@
         <v>25</v>
       </c>
       <c r="E32">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="F32">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="G32">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>100</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
@@ -1427,14 +1427,14 @@
         <v>15</v>
       </c>
       <c r="E33">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="F33">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="G33">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>100</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
@@ -1451,14 +1451,14 @@
         <v>10</v>
       </c>
       <c r="E34">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="F34">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="G34">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>100</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
@@ -1475,14 +1475,14 @@
         <v>10</v>
       </c>
       <c r="E35">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="F35">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="G35">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>100</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
@@ -1499,14 +1499,14 @@
         <v>10</v>
       </c>
       <c r="E36">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="F36">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="G36">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>100</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
@@ -1523,14 +1523,14 @@
         <v>5</v>
       </c>
       <c r="E37">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="F37">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="G37">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>100</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>